<commit_message>
[Fix] 개선사항 적용 (#101)
1. 마을 오브젝트 메쉬 콜라이더 적용
2. 마법사 퀘스트 진행 마크 적용
3. 튜토리얼 UI 수정
4. 매터리얼 수정
5. 퀘스트 UI현황판 몬스터 이름으로 변경
6. 경비병 엔피시id 수정
7. 터레인 일부 수정
8. 검술교관 미니게임 성공 시 이펙트 발생
</commit_message>
<xml_diff>
--- a/Assets/DB/ServeQuestDB.xlsx
+++ b/Assets/DB/ServeQuestDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalProject\Assets\ExcelFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalBuild\Assets\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C67E49-00E4-4273-B5B8-B9B9A76DE6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5364C-6AC1-4292-A1B5-CE6EC0F8B6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21555" windowHeight="11385" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
+    <workbookView xWindow="0" yWindow="1245" windowWidth="21555" windowHeight="11385" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1071,11 +1071,11 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
-        <v>10202002</v>
+      <c r="F3">
+        <v>10114101</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1162,12 +1162,8 @@
       <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="L5" s="1">
-        <v>2</v>
-      </c>
-      <c r="M5" s="1">
-        <v>5</v>
-      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="1">
         <v>10114101</v>
       </c>
@@ -1339,7 +1335,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="J10">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>11</v>
@@ -1508,6 +1504,12 @@
         <v>67</v>
       </c>
       <c r="F15" s="1"/>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
       <c r="N15" s="1">
         <v>10114102</v>
       </c>
@@ -1535,6 +1537,12 @@
         <v>68</v>
       </c>
       <c r="F16" s="1"/>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
@@ -1562,6 +1570,12 @@
         <v>68</v>
       </c>
       <c r="F17" s="1"/>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
       <c r="N17" s="1">
         <v>0</v>
       </c>
@@ -1589,6 +1603,12 @@
         <v>74</v>
       </c>
       <c r="F18" s="1"/>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
       <c r="N18" s="1">
         <v>0</v>
       </c>
@@ -1648,6 +1668,12 @@
         <v>82</v>
       </c>
       <c r="F20" s="1"/>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
[Fix] 개선사항 수정 (#129)
* [Fix] 개선사항 수정

1. 데이 사이클 조정
2. 대기 기능 사용시 npc 이동
3. NPC 속도 수정
4. NavMesh Volume 오브젝트 추가
5. 차원문 이름 수정 및 대화 지문 추가
6. 카메라에 콜라이더
7. 마법사 대화지문에 환경요소 활용 필요 구문 추가
8. 유물 이미지 누락 추가

* Update MainScene.unity

* Update MainScene.unity
</commit_message>
<xml_diff>
--- a/Assets/DB/ServeQuestDB.xlsx
+++ b/Assets/DB/ServeQuestDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalBuild\Assets\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9775B111-73BA-4D23-8F46-E0AA655ED3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF5CAA-B154-4E4D-9D0B-127FE970341F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
+    <workbookView xWindow="4170" yWindow="1395" windowWidth="21555" windowHeight="11385" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1681,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>10161000</v>
       </c>
       <c r="P20" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
[Fix] Bug Fix - KKH
1. 유물먼저 습득 후 대화 시  프리징 현상 픽스
2. 3번 미니게임 버그 픽스
3. NPC 무한 대화 픽스
4. 퀘스트 UI 이상 현상 픽스
</commit_message>
<xml_diff>
--- a/Assets/DB/ServeQuestDB.xlsx
+++ b/Assets/DB/ServeQuestDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalBuild\Assets\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA4F85-F5AC-4378-8F2F-FA452B2F86CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09848C-74E9-4C30-B583-41F52A24A072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
+    <workbookView xWindow="4170" yWindow="1395" windowWidth="21555" windowHeight="11385" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -935,7 +935,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1367,7 +1367,7 @@
         <v>71</v>
       </c>
       <c r="F11" s="1">
-        <v>10202008</v>
+        <v>10102008</v>
       </c>
       <c r="G11">
         <v>1</v>

</xml_diff>

<commit_message>
[Fix] Bug Fix - KKH (#157)
1. 유물먼저 습득 후 대화 시  프리징 현상 픽스
2. 3번 미니게임 버그 픽스
3. NPC 무한 대화 픽스
4. 퀘스트 UI 이상 현상 픽스
</commit_message>
<xml_diff>
--- a/Assets/DB/ServeQuestDB.xlsx
+++ b/Assets/DB/ServeQuestDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalBuild\Assets\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA4F85-F5AC-4378-8F2F-FA452B2F86CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09848C-74E9-4C30-B583-41F52A24A072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
+    <workbookView xWindow="4170" yWindow="1395" windowWidth="21555" windowHeight="11385" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -935,7 +935,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1367,7 +1367,7 @@
         <v>71</v>
       </c>
       <c r="F11" s="1">
-        <v>10202008</v>
+        <v>10102008</v>
       </c>
       <c r="G11">
         <v>1</v>

</xml_diff>